<commit_message>
adjusted PD stent calculation
</commit_message>
<xml_diff>
--- a/PEPRISC Val Data PRELIM.xlsx
+++ b/PEPRISC Val Data PRELIM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sambhav/Desktop/pepConsulting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0FD5CF-EDEE-5D48-8750-FF518E9CD110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77A9904-5A9F-6148-B4A2-927850D37051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -648,9 +648,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -688,9 +688,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,26 +723,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,26 +758,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -971,7 +937,7 @@
   <dimension ref="A1:AF136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>